<commit_message>
data persistence for api dd
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
@@ -142,6 +142,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -263,6 +267,10 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -384,6 +392,10 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -581,7 +593,7 @@
     <t xml:space="preserve">Scoala particulara Little piggie</t>
   </si>
   <si>
-    <t xml:space="preserve">littlepiggie16@automation.33mail.com</t>
+    <t xml:space="preserve">littlepiggie47@automation.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">str Morariei nr 101</t>
@@ -857,7 +869,7 @@
     <t xml:space="preserve">Scolpol Maria</t>
   </si>
   <si>
-    <t xml:space="preserve">marilenaben7@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">marilenaben16@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555112</t>
@@ -1432,8 +1444,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.5587044534413"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.5951417004049"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.1417004048583"/>
   </cols>
@@ -1509,7 +1521,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1684,13 +1696,13 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -2080,8 +2092,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8825910931174"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>

</xml_diff>

<commit_message>
data driven api persistence
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
@@ -146,6 +146,22 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -271,6 +287,22 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -396,6 +428,22 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -593,7 +641,7 @@
     <t xml:space="preserve">Scoala particulara Little piggie</t>
   </si>
   <si>
-    <t xml:space="preserve">littlepiggie47@automation.33mail.com</t>
+    <t xml:space="preserve">littlepiggie63@automation.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">str Morariei nr 101</t>
@@ -869,7 +917,7 @@
     <t xml:space="preserve">Scolpol Maria</t>
   </si>
   <si>
-    <t xml:space="preserve">marilenaben16@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">marilenaben31@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555112</t>
@@ -884,7 +932,7 @@
     <t xml:space="preserve">Mobutu seseku</t>
   </si>
   <si>
-    <t xml:space="preserve">ideaforkih2@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">ideaforkih7@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264111887</t>
@@ -893,7 +941,7 @@
     <t xml:space="preserve">Moceal Rapil</t>
   </si>
   <si>
-    <t xml:space="preserve">boomsie4s2@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">boomsie4s57@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0265444112</t>
@@ -902,7 +950,7 @@
     <t xml:space="preserve">Spiral Agar</t>
   </si>
   <si>
-    <t xml:space="preserve">ocarinass2@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">ocarinass56@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">10:00-21:00</t>
@@ -1444,8 +1492,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.5951417004049"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.0566801619433"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.1417004048583"/>
   </cols>
@@ -1513,7 +1561,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1521,7 +1569,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1696,13 +1744,13 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="N34" activeCellId="0" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -2087,13 +2135,13 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.3481781376518"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>

</xml_diff>

<commit_message>
set Calendis passw for all new business api accounts
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -162,6 +162,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -303,6 +304,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -444,6 +446,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -641,7 +644,7 @@
     <t xml:space="preserve">Scoala particulara Little piggie</t>
   </si>
   <si>
-    <t xml:space="preserve">littlepiggie63@automation.33mail.com</t>
+    <t xml:space="preserve">littlepiggie64@automation.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">str Morariei nr 101</t>
@@ -917,7 +920,7 @@
     <t xml:space="preserve">Scolpol Maria</t>
   </si>
   <si>
-    <t xml:space="preserve">marilenaben31@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">marilenaben32@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555112</t>
@@ -932,7 +935,7 @@
     <t xml:space="preserve">Mobutu seseku</t>
   </si>
   <si>
-    <t xml:space="preserve">ideaforkih7@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">ideaforkih8@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264111887</t>
@@ -941,7 +944,7 @@
     <t xml:space="preserve">Moceal Rapil</t>
   </si>
   <si>
-    <t xml:space="preserve">boomsie4s57@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">boomsie4s58@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0265444112</t>
@@ -950,7 +953,7 @@
     <t xml:space="preserve">Spiral Agar</t>
   </si>
   <si>
-    <t xml:space="preserve">ocarinass56@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">ocarinass57@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">10:00-21:00</t>
@@ -1284,7 +1287,7 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1492,8 +1495,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.0566801619433"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.7004048582996"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.1417004048583"/>
   </cols>
@@ -1561,7 +1564,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1569,7 +1572,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -1750,7 +1753,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.1417004048583"/>
   </cols>
   <sheetData>
@@ -2134,14 +2137,14 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.668016194332"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>

</xml_diff>

<commit_message>
changes on sanity tests
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -146,6 +146,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -271,6 +273,8 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -396,6 +400,8 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -422,7 +428,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -446,7 +452,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -460,7 +466,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -474,7 +480,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">*serviciile trebuie sa apartina neaparat de un domeniu</t>
+          <t>*serviciile trebuie sa apartina neaparat de un domeniu</t>
         </r>
       </text>
     </comment>
@@ -498,7 +504,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">* se pot adauga oricate conturi de angajati doriti</t>
+          <t>* se pot adauga oricate conturi de angajati doriti</t>
         </r>
       </text>
     </comment>
@@ -509,442 +515,442 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="146">
   <si>
-    <t xml:space="preserve">Categorie Afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume Afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email Cont Administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresa afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medicină dentară</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frumusețe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Larissa's style</t>
-  </si>
-  <si>
-    <t xml:space="preserve">larissa@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calea Martirilor 127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0263221114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medicină</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animale de companie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sport și agrement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terapii complementare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instalații</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regomart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regomart@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Piata Mare 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juridic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resurse umane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asigurări</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modă și îmbrăcăminte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organizare evenimente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moda si imbracaminte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scoala particulara Little piggie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">littlepiggie47@automation.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Morariei nr 101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264888641</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imobiliare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bebeco Adeco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bebbeco@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aleea Bucura 46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0254888777</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reparații</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psihologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Altă categorie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rubarba Mihaelaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lilanna1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venula Mihaila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moraritza22@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0261111222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NilaStefania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rimmelplus1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0268774112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresa locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Judet locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Localitate locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miercuri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vineri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sambata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duminica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Str Fraternitatii nr 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluj-Napoca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Flying</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-20:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-14:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inchis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Coloar 89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alba Iulia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0263555441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Alba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-17:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-21:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-15:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Alexadru Mircea nr 69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0254111222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Romulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-12:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-19:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-18:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume domeniu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Locatia domeniului</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scoala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">playing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">art activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Educație</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bronzare organica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chirurgie estetica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coafor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cosmetica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epilare definitiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frizerie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manichiura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masaj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedichiura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remodelare corporala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tatuaje&amp;piercing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Domeniul asociat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durata serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pret serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persoane serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teme acasa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pictura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jocuri logica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100.66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serviciu asignat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scolpol Maria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marilenaben16@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-13:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-17:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobutu seseku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ideaforkih2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264111887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moceal Rapil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boomsie4s2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0265444112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spiral Agar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ocarinass2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-21:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-18:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creare programari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in viitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in trecut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vizualizare calendar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creare programari alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in viitor alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in trecut alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date de contact clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vizualizare baza de date clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editare informatii clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setari orar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setari exceptii</t>
+    <t>Categorie Afacere</t>
+  </si>
+  <si>
+    <t>Nume Afacere</t>
+  </si>
+  <si>
+    <t>Email Cont Administrator</t>
+  </si>
+  <si>
+    <t>Adresa afacere</t>
+  </si>
+  <si>
+    <t>Telefon afacere</t>
+  </si>
+  <si>
+    <t>Medicină dentară</t>
+  </si>
+  <si>
+    <t>Frumusețe</t>
+  </si>
+  <si>
+    <t>Larissa's style</t>
+  </si>
+  <si>
+    <t>larissa@yopmail.com</t>
+  </si>
+  <si>
+    <t>Calea Martirilor 127</t>
+  </si>
+  <si>
+    <t>0263221114</t>
+  </si>
+  <si>
+    <t>Medicină</t>
+  </si>
+  <si>
+    <t>Animale de companie</t>
+  </si>
+  <si>
+    <t>Sport și agrement</t>
+  </si>
+  <si>
+    <t>Terapii complementare</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Instalații</t>
+  </si>
+  <si>
+    <t>Regomart</t>
+  </si>
+  <si>
+    <t>regomart@yopmail.com</t>
+  </si>
+  <si>
+    <t>Piata Mare 45</t>
+  </si>
+  <si>
+    <t>0264555113</t>
+  </si>
+  <si>
+    <t>Juridic</t>
+  </si>
+  <si>
+    <t>Resurse umane</t>
+  </si>
+  <si>
+    <t>Asigurări</t>
+  </si>
+  <si>
+    <t>Modă și îmbrăcăminte</t>
+  </si>
+  <si>
+    <t>Organizare evenimente</t>
+  </si>
+  <si>
+    <t>Moda si imbracaminte</t>
+  </si>
+  <si>
+    <t>Scoala particulara Little piggie</t>
+  </si>
+  <si>
+    <t>littlepiglet48@automation.33mail.com</t>
+  </si>
+  <si>
+    <t>str Morariei nr 101</t>
+  </si>
+  <si>
+    <t>0264888641</t>
+  </si>
+  <si>
+    <t>Imobiliare</t>
+  </si>
+  <si>
+    <t>Bebeco Adeco</t>
+  </si>
+  <si>
+    <t>bebbeco@yopmail.com</t>
+  </si>
+  <si>
+    <t>Aleea Bucura 46</t>
+  </si>
+  <si>
+    <t>0254888777</t>
+  </si>
+  <si>
+    <t>Reparații</t>
+  </si>
+  <si>
+    <t>Psihologie</t>
+  </si>
+  <si>
+    <t>Altă categorie</t>
+  </si>
+  <si>
+    <t>Nume receptionist</t>
+  </si>
+  <si>
+    <t>Email receptionist</t>
+  </si>
+  <si>
+    <t>Telefon receptionist</t>
+  </si>
+  <si>
+    <t>Rubarba Mihaelaa</t>
+  </si>
+  <si>
+    <t>lilanna1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264555887</t>
+  </si>
+  <si>
+    <t>Venula Mihaila</t>
+  </si>
+  <si>
+    <t>moraritza22@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0261111222</t>
+  </si>
+  <si>
+    <t>NilaStefania</t>
+  </si>
+  <si>
+    <t>rimmelplus1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0268774112</t>
+  </si>
+  <si>
+    <t>Adresa locatie</t>
+  </si>
+  <si>
+    <t>Judet locatie</t>
+  </si>
+  <si>
+    <t>Localitate locatie</t>
+  </si>
+  <si>
+    <t>Telefon locatie</t>
+  </si>
+  <si>
+    <t>Nume locatie</t>
+  </si>
+  <si>
+    <t>Luni</t>
+  </si>
+  <si>
+    <t>Marti</t>
+  </si>
+  <si>
+    <t>Miercuri</t>
+  </si>
+  <si>
+    <t>Joi</t>
+  </si>
+  <si>
+    <t>Vineri</t>
+  </si>
+  <si>
+    <t>Sambata</t>
+  </si>
+  <si>
+    <t>Duminica</t>
+  </si>
+  <si>
+    <t>Str Fraternitatii nr 7</t>
+  </si>
+  <si>
+    <t>Cluj</t>
+  </si>
+  <si>
+    <t>Cluj-Napoca</t>
+  </si>
+  <si>
+    <t>0264555141</t>
+  </si>
+  <si>
+    <t>Sediu Flying</t>
+  </si>
+  <si>
+    <t>10:00-20:00</t>
+  </si>
+  <si>
+    <t>10:00-14:00</t>
+  </si>
+  <si>
+    <t>inchis</t>
+  </si>
+  <si>
+    <t>str Coloar 89</t>
+  </si>
+  <si>
+    <t>Alba</t>
+  </si>
+  <si>
+    <t>Alba Iulia</t>
+  </si>
+  <si>
+    <t>0263555441</t>
+  </si>
+  <si>
+    <t>Sediu Alba</t>
+  </si>
+  <si>
+    <t>9:00-17:00</t>
+  </si>
+  <si>
+    <t>9:00-21:00</t>
+  </si>
+  <si>
+    <t>9:00-15:00</t>
+  </si>
+  <si>
+    <t>str Alexadru Mircea nr 69</t>
+  </si>
+  <si>
+    <t>0254111222</t>
+  </si>
+  <si>
+    <t>Sediu Romulus</t>
+  </si>
+  <si>
+    <t>9:00-12:00</t>
+  </si>
+  <si>
+    <t>10:00-19:00</t>
+  </si>
+  <si>
+    <t>10:00-18:00</t>
+  </si>
+  <si>
+    <t>Nume domeniu</t>
+  </si>
+  <si>
+    <t>Locatia domeniului</t>
+  </si>
+  <si>
+    <t>scoala</t>
+  </si>
+  <si>
+    <t>playing</t>
+  </si>
+  <si>
+    <t>art activities</t>
+  </si>
+  <si>
+    <t>Educație</t>
+  </si>
+  <si>
+    <t>Bronzare organica</t>
+  </si>
+  <si>
+    <t>Chirurgie estetica</t>
+  </si>
+  <si>
+    <t>Coafor</t>
+  </si>
+  <si>
+    <t>Cosmetica</t>
+  </si>
+  <si>
+    <t>Epilare definitiva</t>
+  </si>
+  <si>
+    <t>Frizerie</t>
+  </si>
+  <si>
+    <t>Make-up</t>
+  </si>
+  <si>
+    <t>Manichiura</t>
+  </si>
+  <si>
+    <t>Masaj</t>
+  </si>
+  <si>
+    <t>Pedichiura</t>
+  </si>
+  <si>
+    <t>Remodelare corporala</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Spa</t>
+  </si>
+  <si>
+    <t>Tatuaje&amp;piercing</t>
+  </si>
+  <si>
+    <t>Domeniul asociat</t>
+  </si>
+  <si>
+    <t>Serviciu</t>
+  </si>
+  <si>
+    <t>Durata serviciu</t>
+  </si>
+  <si>
+    <t>Pret serviciu</t>
+  </si>
+  <si>
+    <t>Persoane serviciu</t>
+  </si>
+  <si>
+    <t>teme acasa</t>
+  </si>
+  <si>
+    <t>darts</t>
+  </si>
+  <si>
+    <t>pictura</t>
+  </si>
+  <si>
+    <t>jocuri logica</t>
+  </si>
+  <si>
+    <t>100.66</t>
+  </si>
+  <si>
+    <t>Nume angajat</t>
+  </si>
+  <si>
+    <t>Email angajat</t>
+  </si>
+  <si>
+    <t>Telefon angajat</t>
+  </si>
+  <si>
+    <t>Serviciu asignat</t>
+  </si>
+  <si>
+    <t>Scolpol Maria</t>
+  </si>
+  <si>
+    <t>marilenajoom17@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264555112</t>
+  </si>
+  <si>
+    <t>9:00-13:00</t>
+  </si>
+  <si>
+    <t>10:00-17:00</t>
+  </si>
+  <si>
+    <t>Mobutu seseku</t>
+  </si>
+  <si>
+    <t>ideaforkih2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264111887</t>
+  </si>
+  <si>
+    <t>Moceal Rapil</t>
+  </si>
+  <si>
+    <t>boomsie4s2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0265444112</t>
+  </si>
+  <si>
+    <t>Spiral Agar</t>
+  </si>
+  <si>
+    <t>ocarinass2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>10:00-21:00</t>
+  </si>
+  <si>
+    <t>9:00-18:30</t>
+  </si>
+  <si>
+    <t>Creare programari</t>
+  </si>
+  <si>
+    <t>Modificari programari in viitor</t>
+  </si>
+  <si>
+    <t>Modificari programari in trecut</t>
+  </si>
+  <si>
+    <t>Vizualizare calendar</t>
+  </si>
+  <si>
+    <t>Creare programari alti specialisti</t>
+  </si>
+  <si>
+    <t>Modificari programari in viitor alti specialisti</t>
+  </si>
+  <si>
+    <t>Modificari programari in trecut alti specialisti</t>
+  </si>
+  <si>
+    <t>Date de contact clienti</t>
+  </si>
+  <si>
+    <t>Vizualizare baza de date clienti</t>
+  </si>
+  <si>
+    <t>Editare informatii clienti</t>
+  </si>
+  <si>
+    <t>Setari orar</t>
+  </si>
+  <si>
+    <t>Setari exceptii</t>
   </si>
 </sst>
 </file>
@@ -952,7 +958,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
@@ -1151,7 +1157,6 @@
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1236,16 +1241,16 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1444,10 +1449,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.5951417004049"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,16 +1518,16 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1701,9 +1706,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,7 +1808,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1961,13 +1966,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2086,18 +2091,18 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.5263157894737"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8825910931174"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2299,9 +2304,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.35627530364373"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">

</xml_diff>

<commit_message>
repaired api create business account
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -148,6 +148,11 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -275,6 +280,11 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -402,6 +412,11 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -428,7 +443,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Domeniu principal</t>
+          <t xml:space="preserve">Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -452,7 +467,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Domeniu principal</t>
+          <t xml:space="preserve">Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -466,7 +481,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Domeniu principal</t>
+          <t xml:space="preserve">Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -480,7 +495,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>*serviciile trebuie sa apartina neaparat de un domeniu</t>
+          <t xml:space="preserve">*serviciile trebuie sa apartina neaparat de un domeniu</t>
         </r>
       </text>
     </comment>
@@ -504,7 +519,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>* se pot adauga oricate conturi de angajati doriti</t>
+          <t xml:space="preserve">* se pot adauga oricate conturi de angajati doriti</t>
         </r>
       </text>
     </comment>
@@ -515,442 +530,442 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="146">
   <si>
-    <t>Categorie Afacere</t>
-  </si>
-  <si>
-    <t>Nume Afacere</t>
-  </si>
-  <si>
-    <t>Email Cont Administrator</t>
-  </si>
-  <si>
-    <t>Adresa afacere</t>
-  </si>
-  <si>
-    <t>Telefon afacere</t>
-  </si>
-  <si>
-    <t>Medicină dentară</t>
-  </si>
-  <si>
-    <t>Frumusețe</t>
-  </si>
-  <si>
-    <t>Larissa's style</t>
-  </si>
-  <si>
-    <t>larissa@yopmail.com</t>
-  </si>
-  <si>
-    <t>Calea Martirilor 127</t>
-  </si>
-  <si>
-    <t>0263221114</t>
-  </si>
-  <si>
-    <t>Medicină</t>
-  </si>
-  <si>
-    <t>Animale de companie</t>
-  </si>
-  <si>
-    <t>Sport și agrement</t>
-  </si>
-  <si>
-    <t>Terapii complementare</t>
-  </si>
-  <si>
-    <t>Auto</t>
-  </si>
-  <si>
-    <t>Instalații</t>
-  </si>
-  <si>
-    <t>Regomart</t>
-  </si>
-  <si>
-    <t>regomart@yopmail.com</t>
-  </si>
-  <si>
-    <t>Piata Mare 45</t>
-  </si>
-  <si>
-    <t>0264555113</t>
-  </si>
-  <si>
-    <t>Juridic</t>
-  </si>
-  <si>
-    <t>Resurse umane</t>
-  </si>
-  <si>
-    <t>Asigurări</t>
-  </si>
-  <si>
-    <t>Modă și îmbrăcăminte</t>
-  </si>
-  <si>
-    <t>Organizare evenimente</t>
-  </si>
-  <si>
-    <t>Moda si imbracaminte</t>
-  </si>
-  <si>
-    <t>Scoala particulara Little piggie</t>
-  </si>
-  <si>
-    <t>littlepiglet48@automation.33mail.com</t>
-  </si>
-  <si>
-    <t>str Morariei nr 101</t>
-  </si>
-  <si>
-    <t>0264888641</t>
-  </si>
-  <si>
-    <t>Imobiliare</t>
-  </si>
-  <si>
-    <t>Bebeco Adeco</t>
-  </si>
-  <si>
-    <t>bebbeco@yopmail.com</t>
-  </si>
-  <si>
-    <t>Aleea Bucura 46</t>
-  </si>
-  <si>
-    <t>0254888777</t>
-  </si>
-  <si>
-    <t>Reparații</t>
-  </si>
-  <si>
-    <t>Psihologie</t>
-  </si>
-  <si>
-    <t>Altă categorie</t>
-  </si>
-  <si>
-    <t>Nume receptionist</t>
-  </si>
-  <si>
-    <t>Email receptionist</t>
-  </si>
-  <si>
-    <t>Telefon receptionist</t>
-  </si>
-  <si>
-    <t>Rubarba Mihaelaa</t>
-  </si>
-  <si>
-    <t>lilanna1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0264555887</t>
-  </si>
-  <si>
-    <t>Venula Mihaila</t>
-  </si>
-  <si>
-    <t>moraritza22@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0261111222</t>
-  </si>
-  <si>
-    <t>NilaStefania</t>
-  </si>
-  <si>
-    <t>rimmelplus1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0268774112</t>
-  </si>
-  <si>
-    <t>Adresa locatie</t>
-  </si>
-  <si>
-    <t>Judet locatie</t>
-  </si>
-  <si>
-    <t>Localitate locatie</t>
-  </si>
-  <si>
-    <t>Telefon locatie</t>
-  </si>
-  <si>
-    <t>Nume locatie</t>
-  </si>
-  <si>
-    <t>Luni</t>
-  </si>
-  <si>
-    <t>Marti</t>
-  </si>
-  <si>
-    <t>Miercuri</t>
-  </si>
-  <si>
-    <t>Joi</t>
-  </si>
-  <si>
-    <t>Vineri</t>
-  </si>
-  <si>
-    <t>Sambata</t>
-  </si>
-  <si>
-    <t>Duminica</t>
-  </si>
-  <si>
-    <t>Str Fraternitatii nr 7</t>
-  </si>
-  <si>
-    <t>Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Napoca</t>
-  </si>
-  <si>
-    <t>0264555141</t>
-  </si>
-  <si>
-    <t>Sediu Flying</t>
-  </si>
-  <si>
-    <t>10:00-20:00</t>
-  </si>
-  <si>
-    <t>10:00-14:00</t>
-  </si>
-  <si>
-    <t>inchis</t>
-  </si>
-  <si>
-    <t>str Coloar 89</t>
-  </si>
-  <si>
-    <t>Alba</t>
-  </si>
-  <si>
-    <t>Alba Iulia</t>
-  </si>
-  <si>
-    <t>0263555441</t>
-  </si>
-  <si>
-    <t>Sediu Alba</t>
-  </si>
-  <si>
-    <t>9:00-17:00</t>
-  </si>
-  <si>
-    <t>9:00-21:00</t>
-  </si>
-  <si>
-    <t>9:00-15:00</t>
-  </si>
-  <si>
-    <t>str Alexadru Mircea nr 69</t>
-  </si>
-  <si>
-    <t>0254111222</t>
-  </si>
-  <si>
-    <t>Sediu Romulus</t>
-  </si>
-  <si>
-    <t>9:00-12:00</t>
-  </si>
-  <si>
-    <t>10:00-19:00</t>
-  </si>
-  <si>
-    <t>10:00-18:00</t>
-  </si>
-  <si>
-    <t>Nume domeniu</t>
-  </si>
-  <si>
-    <t>Locatia domeniului</t>
-  </si>
-  <si>
-    <t>scoala</t>
-  </si>
-  <si>
-    <t>playing</t>
-  </si>
-  <si>
-    <t>art activities</t>
-  </si>
-  <si>
-    <t>Educație</t>
-  </si>
-  <si>
-    <t>Bronzare organica</t>
-  </si>
-  <si>
-    <t>Chirurgie estetica</t>
-  </si>
-  <si>
-    <t>Coafor</t>
-  </si>
-  <si>
-    <t>Cosmetica</t>
-  </si>
-  <si>
-    <t>Epilare definitiva</t>
-  </si>
-  <si>
-    <t>Frizerie</t>
-  </si>
-  <si>
-    <t>Make-up</t>
-  </si>
-  <si>
-    <t>Manichiura</t>
-  </si>
-  <si>
-    <t>Masaj</t>
-  </si>
-  <si>
-    <t>Pedichiura</t>
-  </si>
-  <si>
-    <t>Remodelare corporala</t>
-  </si>
-  <si>
-    <t>Solar</t>
-  </si>
-  <si>
-    <t>Spa</t>
-  </si>
-  <si>
-    <t>Tatuaje&amp;piercing</t>
-  </si>
-  <si>
-    <t>Domeniul asociat</t>
-  </si>
-  <si>
-    <t>Serviciu</t>
-  </si>
-  <si>
-    <t>Durata serviciu</t>
-  </si>
-  <si>
-    <t>Pret serviciu</t>
-  </si>
-  <si>
-    <t>Persoane serviciu</t>
-  </si>
-  <si>
-    <t>teme acasa</t>
-  </si>
-  <si>
-    <t>darts</t>
-  </si>
-  <si>
-    <t>pictura</t>
-  </si>
-  <si>
-    <t>jocuri logica</t>
-  </si>
-  <si>
-    <t>100.66</t>
-  </si>
-  <si>
-    <t>Nume angajat</t>
-  </si>
-  <si>
-    <t>Email angajat</t>
-  </si>
-  <si>
-    <t>Telefon angajat</t>
-  </si>
-  <si>
-    <t>Serviciu asignat</t>
-  </si>
-  <si>
-    <t>Scolpol Maria</t>
-  </si>
-  <si>
-    <t>marilenajoom17@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0264555112</t>
-  </si>
-  <si>
-    <t>9:00-13:00</t>
-  </si>
-  <si>
-    <t>10:00-17:00</t>
-  </si>
-  <si>
-    <t>Mobutu seseku</t>
-  </si>
-  <si>
-    <t>ideaforkih2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0264111887</t>
-  </si>
-  <si>
-    <t>Moceal Rapil</t>
-  </si>
-  <si>
-    <t>boomsie4s2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>0265444112</t>
-  </si>
-  <si>
-    <t>Spiral Agar</t>
-  </si>
-  <si>
-    <t>ocarinass2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t>10:00-21:00</t>
-  </si>
-  <si>
-    <t>9:00-18:30</t>
-  </si>
-  <si>
-    <t>Creare programari</t>
-  </si>
-  <si>
-    <t>Modificari programari in viitor</t>
-  </si>
-  <si>
-    <t>Modificari programari in trecut</t>
-  </si>
-  <si>
-    <t>Vizualizare calendar</t>
-  </si>
-  <si>
-    <t>Creare programari alti specialisti</t>
-  </si>
-  <si>
-    <t>Modificari programari in viitor alti specialisti</t>
-  </si>
-  <si>
-    <t>Modificari programari in trecut alti specialisti</t>
-  </si>
-  <si>
-    <t>Date de contact clienti</t>
-  </si>
-  <si>
-    <t>Vizualizare baza de date clienti</t>
-  </si>
-  <si>
-    <t>Editare informatii clienti</t>
-  </si>
-  <si>
-    <t>Setari orar</t>
-  </si>
-  <si>
-    <t>Setari exceptii</t>
+    <t xml:space="preserve">Categorie Afacere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume Afacere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Cont Administrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresa afacere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefon afacere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medicină dentară</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frumusețe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larissa's style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">larissa@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calea Martirilor 127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0263221114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medicină</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animale de companie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sport și agrement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terapii complementare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instalații</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regomart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regomart@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piata Mare 45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264555113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juridic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resurse umane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asigurări</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modă și îmbrăcăminte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organizare evenimente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moda si imbracaminte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scoala particulara Little piggie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">littlepiglet54@automation.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str Morariei nr 101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264888641</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imobiliare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bebeco Adeco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bebbeco@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aleea Bucura 46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0254888777</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reparații</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psihologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altă categorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume receptionist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email receptionist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefon receptionist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rubarba Mihaelaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lilanna1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264555887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venula Mihaila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moraritza22@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0261111222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NilaStefania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rimmelplus1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0268774112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresa locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Judet locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Localitate locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefon locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume locatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miercuri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vineri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sambata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duminica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Str Fraternitatii nr 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluj-Napoca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264555141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediu Flying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-20:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-14:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inchis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str Coloar 89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alba Iulia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0263555441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediu Alba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-21:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-15:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str Alexadru Mircea nr 69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0254111222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sediu Romulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-12:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-19:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume domeniu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locatia domeniului</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scoala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">playing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">art activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Educație</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bronzare organica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chirurgie estetica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coafor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cosmetica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epilare definitiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frizerie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make-up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manichiura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masaj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedichiura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remodelare corporala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tatuaje&amp;piercing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domeniul asociat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serviciu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durata serviciu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pret serviciu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persoane serviciu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teme acasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">darts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pictura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jocuri logica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100.66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nume angajat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email angajat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefon angajat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serviciu asignat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scolpol Maria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marilenajoom23@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264555112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-13:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobutu seseku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ideaforkih2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0264111887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moceal Rapil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boomsie4s2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0265444112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spiral Agar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ocarinass2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00-21:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:00-18:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creare programari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificari programari in viitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificari programari in trecut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vizualizare calendar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creare programari alti specialisti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificari programari in viitor alti specialisti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificari programari in trecut alti specialisti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date de contact clienti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vizualizare baza de date clienti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editare informatii clienti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setari orar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setari exceptii</t>
   </si>
 </sst>
 </file>
@@ -958,7 +973,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
@@ -1157,6 +1172,7 @@
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1241,16 +1257,16 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.03238866396761"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1449,10 +1465,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.663967611336"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1523,11 +1539,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,9 +1722,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,7 +1824,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1966,13 +1982,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.24696356275304"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.10526315789474"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.24696356275304"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2091,18 +2107,18 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.03238866396761"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2304,6 +2320,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">

</xml_diff>

<commit_message>
collect payment for packet test refactor
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -153,6 +153,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -285,6 +287,8 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -417,6 +421,8 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -443,7 +449,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -467,7 +473,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -481,7 +487,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -495,7 +501,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">*serviciile trebuie sa apartina neaparat de un domeniu</t>
+          <t>*serviciile trebuie sa apartina neaparat de un domeniu</t>
         </r>
       </text>
     </comment>
@@ -519,7 +525,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">* se pot adauga oricate conturi de angajati doriti</t>
+          <t>* se pot adauga oricate conturi de angajati doriti</t>
         </r>
       </text>
     </comment>
@@ -530,442 +536,442 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="146">
   <si>
-    <t xml:space="preserve">Categorie Afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume Afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email Cont Administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresa afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medicină dentară</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frumusețe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Larissa's style</t>
-  </si>
-  <si>
-    <t xml:space="preserve">larissa@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calea Martirilor 127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0263221114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medicină</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animale de companie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sport și agrement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terapii complementare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instalații</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regomart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regomart@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Piata Mare 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juridic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resurse umane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asigurări</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modă și îmbrăcăminte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organizare evenimente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moda si imbracaminte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scoala particulara Little piggie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">littlepiglet54@automation.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Morariei nr 101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264888641</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imobiliare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bebeco Adeco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bebbeco@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aleea Bucura 46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0254888777</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reparații</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psihologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Altă categorie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rubarba Mihaelaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lilanna1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venula Mihaila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moraritza22@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0261111222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NilaStefania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rimmelplus1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0268774112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresa locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Judet locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Localitate locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miercuri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vineri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sambata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duminica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Str Fraternitatii nr 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluj-Napoca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Flying</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-20:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-14:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inchis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Coloar 89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alba Iulia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0263555441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Alba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-17:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-21:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-15:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Alexadru Mircea nr 69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0254111222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Romulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-12:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-19:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-18:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume domeniu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Locatia domeniului</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scoala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">playing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">art activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Educație</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bronzare organica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chirurgie estetica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coafor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cosmetica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epilare definitiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frizerie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manichiura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masaj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedichiura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remodelare corporala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tatuaje&amp;piercing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Domeniul asociat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durata serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pret serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persoane serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teme acasa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pictura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jocuri logica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100.66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serviciu asignat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scolpol Maria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marilenajoom23@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-13:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-17:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobutu seseku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ideaforkih2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264111887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moceal Rapil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boomsie4s2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0265444112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spiral Agar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ocarinass2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-21:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-18:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creare programari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in viitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in trecut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vizualizare calendar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creare programari alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in viitor alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in trecut alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date de contact clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vizualizare baza de date clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editare informatii clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setari orar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setari exceptii</t>
+    <t>Categorie Afacere</t>
+  </si>
+  <si>
+    <t>Nume Afacere</t>
+  </si>
+  <si>
+    <t>Email Cont Administrator</t>
+  </si>
+  <si>
+    <t>Adresa afacere</t>
+  </si>
+  <si>
+    <t>Telefon afacere</t>
+  </si>
+  <si>
+    <t>Medicină dentară</t>
+  </si>
+  <si>
+    <t>Frumusețe</t>
+  </si>
+  <si>
+    <t>Larissa's style</t>
+  </si>
+  <si>
+    <t>larissa@yopmail.com</t>
+  </si>
+  <si>
+    <t>Calea Martirilor 127</t>
+  </si>
+  <si>
+    <t>0263221114</t>
+  </si>
+  <si>
+    <t>Medicină</t>
+  </si>
+  <si>
+    <t>Animale de companie</t>
+  </si>
+  <si>
+    <t>Sport și agrement</t>
+  </si>
+  <si>
+    <t>Terapii complementare</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Instalații</t>
+  </si>
+  <si>
+    <t>Regomart</t>
+  </si>
+  <si>
+    <t>regomart@yopmail.com</t>
+  </si>
+  <si>
+    <t>Piata Mare 45</t>
+  </si>
+  <si>
+    <t>0264555113</t>
+  </si>
+  <si>
+    <t>Juridic</t>
+  </si>
+  <si>
+    <t>Resurse umane</t>
+  </si>
+  <si>
+    <t>Asigurări</t>
+  </si>
+  <si>
+    <t>Modă și îmbrăcăminte</t>
+  </si>
+  <si>
+    <t>Organizare evenimente</t>
+  </si>
+  <si>
+    <t>Moda si imbracaminte</t>
+  </si>
+  <si>
+    <t>Scoala particulara Little piggie</t>
+  </si>
+  <si>
+    <t>littlepiglfgt55@automation.33mail.com</t>
+  </si>
+  <si>
+    <t>str Morariei nr 101</t>
+  </si>
+  <si>
+    <t>0264888641</t>
+  </si>
+  <si>
+    <t>Imobiliare</t>
+  </si>
+  <si>
+    <t>Bebeco Adeco</t>
+  </si>
+  <si>
+    <t>bebbeco@yopmail.com</t>
+  </si>
+  <si>
+    <t>Aleea Bucura 46</t>
+  </si>
+  <si>
+    <t>0254888777</t>
+  </si>
+  <si>
+    <t>Reparații</t>
+  </si>
+  <si>
+    <t>Psihologie</t>
+  </si>
+  <si>
+    <t>Altă categorie</t>
+  </si>
+  <si>
+    <t>Nume receptionist</t>
+  </si>
+  <si>
+    <t>Email receptionist</t>
+  </si>
+  <si>
+    <t>Telefon receptionist</t>
+  </si>
+  <si>
+    <t>Rubarba Mihaelaa</t>
+  </si>
+  <si>
+    <t>lilanna1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264555887</t>
+  </si>
+  <si>
+    <t>Venula Mihaila</t>
+  </si>
+  <si>
+    <t>moraritza22@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0261111222</t>
+  </si>
+  <si>
+    <t>NilaStefania</t>
+  </si>
+  <si>
+    <t>rimmelplus1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0268774112</t>
+  </si>
+  <si>
+    <t>Adresa locatie</t>
+  </si>
+  <si>
+    <t>Judet locatie</t>
+  </si>
+  <si>
+    <t>Localitate locatie</t>
+  </si>
+  <si>
+    <t>Telefon locatie</t>
+  </si>
+  <si>
+    <t>Nume locatie</t>
+  </si>
+  <si>
+    <t>Luni</t>
+  </si>
+  <si>
+    <t>Marti</t>
+  </si>
+  <si>
+    <t>Miercuri</t>
+  </si>
+  <si>
+    <t>Joi</t>
+  </si>
+  <si>
+    <t>Vineri</t>
+  </si>
+  <si>
+    <t>Sambata</t>
+  </si>
+  <si>
+    <t>Duminica</t>
+  </si>
+  <si>
+    <t>Str Fraternitatii nr 7</t>
+  </si>
+  <si>
+    <t>Cluj</t>
+  </si>
+  <si>
+    <t>Cluj-Napoca</t>
+  </si>
+  <si>
+    <t>0264555141</t>
+  </si>
+  <si>
+    <t>Sediu Flying</t>
+  </si>
+  <si>
+    <t>10:00-20:00</t>
+  </si>
+  <si>
+    <t>10:00-14:00</t>
+  </si>
+  <si>
+    <t>inchis</t>
+  </si>
+  <si>
+    <t>str Coloar 89</t>
+  </si>
+  <si>
+    <t>Alba</t>
+  </si>
+  <si>
+    <t>Alba Iulia</t>
+  </si>
+  <si>
+    <t>0263555441</t>
+  </si>
+  <si>
+    <t>Sediu Alba</t>
+  </si>
+  <si>
+    <t>9:00-17:00</t>
+  </si>
+  <si>
+    <t>9:00-21:00</t>
+  </si>
+  <si>
+    <t>9:00-15:00</t>
+  </si>
+  <si>
+    <t>str Alexadru Mircea nr 69</t>
+  </si>
+  <si>
+    <t>0254111222</t>
+  </si>
+  <si>
+    <t>Sediu Romulus</t>
+  </si>
+  <si>
+    <t>9:00-12:00</t>
+  </si>
+  <si>
+    <t>10:00-19:00</t>
+  </si>
+  <si>
+    <t>10:00-18:00</t>
+  </si>
+  <si>
+    <t>Nume domeniu</t>
+  </si>
+  <si>
+    <t>Locatia domeniului</t>
+  </si>
+  <si>
+    <t>scoala</t>
+  </si>
+  <si>
+    <t>playing</t>
+  </si>
+  <si>
+    <t>art activities</t>
+  </si>
+  <si>
+    <t>Educație</t>
+  </si>
+  <si>
+    <t>Bronzare organica</t>
+  </si>
+  <si>
+    <t>Chirurgie estetica</t>
+  </si>
+  <si>
+    <t>Coafor</t>
+  </si>
+  <si>
+    <t>Cosmetica</t>
+  </si>
+  <si>
+    <t>Epilare definitiva</t>
+  </si>
+  <si>
+    <t>Frizerie</t>
+  </si>
+  <si>
+    <t>Make-up</t>
+  </si>
+  <si>
+    <t>Manichiura</t>
+  </si>
+  <si>
+    <t>Masaj</t>
+  </si>
+  <si>
+    <t>Pedichiura</t>
+  </si>
+  <si>
+    <t>Remodelare corporala</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Spa</t>
+  </si>
+  <si>
+    <t>Tatuaje&amp;piercing</t>
+  </si>
+  <si>
+    <t>Domeniul asociat</t>
+  </si>
+  <si>
+    <t>Serviciu</t>
+  </si>
+  <si>
+    <t>Durata serviciu</t>
+  </si>
+  <si>
+    <t>Pret serviciu</t>
+  </si>
+  <si>
+    <t>Persoane serviciu</t>
+  </si>
+  <si>
+    <t>teme acasa</t>
+  </si>
+  <si>
+    <t>darts</t>
+  </si>
+  <si>
+    <t>pictura</t>
+  </si>
+  <si>
+    <t>jocuri logica</t>
+  </si>
+  <si>
+    <t>100.66</t>
+  </si>
+  <si>
+    <t>Nume angajat</t>
+  </si>
+  <si>
+    <t>Email angajat</t>
+  </si>
+  <si>
+    <t>Telefon angajat</t>
+  </si>
+  <si>
+    <t>Serviciu asignat</t>
+  </si>
+  <si>
+    <t>Scolpol Maria</t>
+  </si>
+  <si>
+    <t>jjjnajoom24@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264555112</t>
+  </si>
+  <si>
+    <t>9:00-13:00</t>
+  </si>
+  <si>
+    <t>10:00-17:00</t>
+  </si>
+  <si>
+    <t>Mobutu seseku</t>
+  </si>
+  <si>
+    <t>ideaforkih2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264111887</t>
+  </si>
+  <si>
+    <t>Moceal Rapil</t>
+  </si>
+  <si>
+    <t>boomsie4s2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0265444112</t>
+  </si>
+  <si>
+    <t>Spiral Agar</t>
+  </si>
+  <si>
+    <t>ocarinass2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>10:00-21:00</t>
+  </si>
+  <si>
+    <t>9:00-18:30</t>
+  </si>
+  <si>
+    <t>Creare programari</t>
+  </si>
+  <si>
+    <t>Modificari programari in viitor</t>
+  </si>
+  <si>
+    <t>Modificari programari in trecut</t>
+  </si>
+  <si>
+    <t>Vizualizare calendar</t>
+  </si>
+  <si>
+    <t>Creare programari alti specialisti</t>
+  </si>
+  <si>
+    <t>Modificari programari in viitor alti specialisti</t>
+  </si>
+  <si>
+    <t>Modificari programari in trecut alti specialisti</t>
+  </si>
+  <si>
+    <t>Date de contact clienti</t>
+  </si>
+  <si>
+    <t>Vizualizare baza de date clienti</t>
+  </si>
+  <si>
+    <t>Editare informatii clienti</t>
+  </si>
+  <si>
+    <t>Setari orar</t>
+  </si>
+  <si>
+    <t>Setari exceptii</t>
   </si>
 </sst>
 </file>
@@ -973,7 +979,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
@@ -1172,7 +1178,6 @@
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1263,10 +1268,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,10 +1470,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.663967611336"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1539,11 +1544,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,9 +1727,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1824,7 +1829,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,13 +1987,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2113,12 +2116,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2321,7 +2324,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
removed capitalize from add voucher test
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
@@ -155,6 +155,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -289,6 +291,8 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -423,6 +427,8 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -620,7 +626,7 @@
     <t>Scoala particulara Little piggie</t>
   </si>
   <si>
-    <t>littlepiglfgt55@automation.33mail.com</t>
+    <t>littlepig99@automation.33mail.com</t>
   </si>
   <si>
     <t>str Morariei nr 101</t>
@@ -896,7 +902,7 @@
     <t>Scolpol Maria</t>
   </si>
   <si>
-    <t>jjjnajoom24@staffcalendis.33mail.com</t>
+    <t>jjjnajoom33@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0264555112</t>
@@ -1268,10 +1274,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1470,10 +1476,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.3163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1544,11 +1549,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,9 +1731,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,9 +1831,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
@@ -1987,11 +1987,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2111,17 +2112,15 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2602040816326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2323,9 +2322,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">

</xml_diff>

<commit_message>
Add business subscription tests
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -153,6 +153,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -285,6 +289,10 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -417,6 +425,10 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -443,7 +455,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -467,7 +479,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -481,7 +493,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Domeniu principal</t>
+          <t>Domeniu principal</t>
         </r>
       </text>
     </comment>
@@ -495,7 +507,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">*serviciile trebuie sa apartina neaparat de un domeniu</t>
+          <t>*serviciile trebuie sa apartina neaparat de un domeniu</t>
         </r>
       </text>
     </comment>
@@ -519,7 +531,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">* se pot adauga oricate conturi de angajati doriti</t>
+          <t>* se pot adauga oricate conturi de angajati doriti</t>
         </r>
       </text>
     </comment>
@@ -530,442 +542,442 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="146">
   <si>
-    <t xml:space="preserve">Categorie Afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume Afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email Cont Administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresa afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon afacere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medicină dentară</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frumusețe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Larissa's style</t>
-  </si>
-  <si>
-    <t xml:space="preserve">larissa@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calea Martirilor 127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0263221114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medicină</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animale de companie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sport și agrement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terapii complementare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instalații</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regomart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regomart@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Piata Mare 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juridic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resurse umane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asigurări</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modă și îmbrăcăminte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organizare evenimente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moda si imbracaminte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scoala particulara Little piggie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">littlepiglet54@automation.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Morariei nr 101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264888641</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imobiliare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bebeco Adeco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bebbeco@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aleea Bucura 46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0254888777</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reparații</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Psihologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Altă categorie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon receptionist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rubarba Mihaelaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lilanna1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venula Mihaila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moraritza22@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0261111222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NilaStefania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rimmelplus1@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0268774112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresa locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Judet locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Localitate locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume locatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miercuri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vineri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sambata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duminica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Str Fraternitatii nr 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cluj-Napoca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Flying</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-20:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-14:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inchis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Coloar 89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alba Iulia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0263555441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Alba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-17:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-21:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-15:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">str Alexadru Mircea nr 69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0254111222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sediu Romulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-12:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-19:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-18:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume domeniu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Locatia domeniului</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scoala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">playing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">art activities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Educație</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bronzare organica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chirurgie estetica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coafor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cosmetica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epilare definitiva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frizerie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manichiura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masaj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedichiura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remodelare corporala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tatuaje&amp;piercing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Domeniul asociat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durata serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pret serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persoane serviciu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teme acasa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">darts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pictura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jocuri logica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100.66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nume angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefon angajat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serviciu asignat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scolpol Maria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marilenajoom23@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264555112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-13:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-17:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobutu seseku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ideaforkih2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0264111887</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moceal Rapil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boomsie4s2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0265444112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spiral Agar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ocarinass2@staffcalendis.33mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:00-21:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9:00-18:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creare programari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in viitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in trecut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vizualizare calendar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creare programari alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in viitor alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modificari programari in trecut alti specialisti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date de contact clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vizualizare baza de date clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editare informatii clienti</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setari orar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setari exceptii</t>
+    <t>Categorie Afacere</t>
+  </si>
+  <si>
+    <t>Nume Afacere</t>
+  </si>
+  <si>
+    <t>Email Cont Administrator</t>
+  </si>
+  <si>
+    <t>Adresa afacere</t>
+  </si>
+  <si>
+    <t>Telefon afacere</t>
+  </si>
+  <si>
+    <t>Medicină dentară</t>
+  </si>
+  <si>
+    <t>Frumusețe</t>
+  </si>
+  <si>
+    <t>Larissa's style</t>
+  </si>
+  <si>
+    <t>larissa@yopmail.com</t>
+  </si>
+  <si>
+    <t>Calea Martirilor 127</t>
+  </si>
+  <si>
+    <t>0263221114</t>
+  </si>
+  <si>
+    <t>Medicină</t>
+  </si>
+  <si>
+    <t>Animale de companie</t>
+  </si>
+  <si>
+    <t>Sport și agrement</t>
+  </si>
+  <si>
+    <t>Terapii complementare</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Instalații</t>
+  </si>
+  <si>
+    <t>Regomart</t>
+  </si>
+  <si>
+    <t>regomart@yopmail.com</t>
+  </si>
+  <si>
+    <t>Piata Mare 45</t>
+  </si>
+  <si>
+    <t>0264555113</t>
+  </si>
+  <si>
+    <t>Juridic</t>
+  </si>
+  <si>
+    <t>Resurse umane</t>
+  </si>
+  <si>
+    <t>Asigurări</t>
+  </si>
+  <si>
+    <t>Modă și îmbrăcăminte</t>
+  </si>
+  <si>
+    <t>Organizare evenimente</t>
+  </si>
+  <si>
+    <t>Moda si imbracaminte</t>
+  </si>
+  <si>
+    <t>Scoala particulara Little piggie</t>
+  </si>
+  <si>
+    <t>littlepiglet58@automation.33mail.com</t>
+  </si>
+  <si>
+    <t>str Morariei nr 101</t>
+  </si>
+  <si>
+    <t>0264888641</t>
+  </si>
+  <si>
+    <t>Imobiliare</t>
+  </si>
+  <si>
+    <t>Bebeco Adeco</t>
+  </si>
+  <si>
+    <t>bebbeco@yopmail.com</t>
+  </si>
+  <si>
+    <t>Aleea Bucura 46</t>
+  </si>
+  <si>
+    <t>0254888777</t>
+  </si>
+  <si>
+    <t>Reparații</t>
+  </si>
+  <si>
+    <t>Psihologie</t>
+  </si>
+  <si>
+    <t>Altă categorie</t>
+  </si>
+  <si>
+    <t>Nume receptionist</t>
+  </si>
+  <si>
+    <t>Email receptionist</t>
+  </si>
+  <si>
+    <t>Telefon receptionist</t>
+  </si>
+  <si>
+    <t>Rubarba Mihaelaa</t>
+  </si>
+  <si>
+    <t>lilanna1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264555887</t>
+  </si>
+  <si>
+    <t>Venula Mihaila</t>
+  </si>
+  <si>
+    <t>moraritza22@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0261111222</t>
+  </si>
+  <si>
+    <t>NilaStefania</t>
+  </si>
+  <si>
+    <t>rimmelplus1@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0268774112</t>
+  </si>
+  <si>
+    <t>Adresa locatie</t>
+  </si>
+  <si>
+    <t>Judet locatie</t>
+  </si>
+  <si>
+    <t>Localitate locatie</t>
+  </si>
+  <si>
+    <t>Telefon locatie</t>
+  </si>
+  <si>
+    <t>Nume locatie</t>
+  </si>
+  <si>
+    <t>Luni</t>
+  </si>
+  <si>
+    <t>Marti</t>
+  </si>
+  <si>
+    <t>Miercuri</t>
+  </si>
+  <si>
+    <t>Joi</t>
+  </si>
+  <si>
+    <t>Vineri</t>
+  </si>
+  <si>
+    <t>Sambata</t>
+  </si>
+  <si>
+    <t>Duminica</t>
+  </si>
+  <si>
+    <t>Str Fraternitatii nr 7</t>
+  </si>
+  <si>
+    <t>Cluj</t>
+  </si>
+  <si>
+    <t>Cluj-Napoca</t>
+  </si>
+  <si>
+    <t>0264555141</t>
+  </si>
+  <si>
+    <t>Sediu Flying</t>
+  </si>
+  <si>
+    <t>10:00-20:00</t>
+  </si>
+  <si>
+    <t>10:00-14:00</t>
+  </si>
+  <si>
+    <t>inchis</t>
+  </si>
+  <si>
+    <t>str Coloar 89</t>
+  </si>
+  <si>
+    <t>Alba</t>
+  </si>
+  <si>
+    <t>Alba Iulia</t>
+  </si>
+  <si>
+    <t>0263555441</t>
+  </si>
+  <si>
+    <t>Sediu Alba</t>
+  </si>
+  <si>
+    <t>9:00-17:00</t>
+  </si>
+  <si>
+    <t>9:00-21:00</t>
+  </si>
+  <si>
+    <t>9:00-15:00</t>
+  </si>
+  <si>
+    <t>str Alexadru Mircea nr 69</t>
+  </si>
+  <si>
+    <t>0254111222</t>
+  </si>
+  <si>
+    <t>Sediu Romulus</t>
+  </si>
+  <si>
+    <t>9:00-12:00</t>
+  </si>
+  <si>
+    <t>10:00-19:00</t>
+  </si>
+  <si>
+    <t>10:00-18:00</t>
+  </si>
+  <si>
+    <t>Nume domeniu</t>
+  </si>
+  <si>
+    <t>Locatia domeniului</t>
+  </si>
+  <si>
+    <t>scoala</t>
+  </si>
+  <si>
+    <t>playing</t>
+  </si>
+  <si>
+    <t>art activities</t>
+  </si>
+  <si>
+    <t>Educație</t>
+  </si>
+  <si>
+    <t>Bronzare organica</t>
+  </si>
+  <si>
+    <t>Chirurgie estetica</t>
+  </si>
+  <si>
+    <t>Coafor</t>
+  </si>
+  <si>
+    <t>Cosmetica</t>
+  </si>
+  <si>
+    <t>Epilare definitiva</t>
+  </si>
+  <si>
+    <t>Frizerie</t>
+  </si>
+  <si>
+    <t>Make-up</t>
+  </si>
+  <si>
+    <t>Manichiura</t>
+  </si>
+  <si>
+    <t>Masaj</t>
+  </si>
+  <si>
+    <t>Pedichiura</t>
+  </si>
+  <si>
+    <t>Remodelare corporala</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>Spa</t>
+  </si>
+  <si>
+    <t>Tatuaje&amp;piercing</t>
+  </si>
+  <si>
+    <t>Domeniul asociat</t>
+  </si>
+  <si>
+    <t>Serviciu</t>
+  </si>
+  <si>
+    <t>Durata serviciu</t>
+  </si>
+  <si>
+    <t>Pret serviciu</t>
+  </si>
+  <si>
+    <t>Persoane serviciu</t>
+  </si>
+  <si>
+    <t>teme acasa</t>
+  </si>
+  <si>
+    <t>darts</t>
+  </si>
+  <si>
+    <t>pictura</t>
+  </si>
+  <si>
+    <t>jocuri logica</t>
+  </si>
+  <si>
+    <t>100.66</t>
+  </si>
+  <si>
+    <t>Nume angajat</t>
+  </si>
+  <si>
+    <t>Email angajat</t>
+  </si>
+  <si>
+    <t>Telefon angajat</t>
+  </si>
+  <si>
+    <t>Serviciu asignat</t>
+  </si>
+  <si>
+    <t>Scolpol Maria</t>
+  </si>
+  <si>
+    <t>marilenajooma26@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264555112</t>
+  </si>
+  <si>
+    <t>9:00-13:00</t>
+  </si>
+  <si>
+    <t>10:00-17:00</t>
+  </si>
+  <si>
+    <t>Mobutu seseku</t>
+  </si>
+  <si>
+    <t>ideaforkih2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0264111887</t>
+  </si>
+  <si>
+    <t>Moceal Rapil</t>
+  </si>
+  <si>
+    <t>boomsie4s2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>0265444112</t>
+  </si>
+  <si>
+    <t>Spiral Agar</t>
+  </si>
+  <si>
+    <t>ocarinass2@staffcalendis.33mail.com</t>
+  </si>
+  <si>
+    <t>10:00-21:00</t>
+  </si>
+  <si>
+    <t>9:00-18:30</t>
+  </si>
+  <si>
+    <t>Creare programari</t>
+  </si>
+  <si>
+    <t>Modificari programari in viitor</t>
+  </si>
+  <si>
+    <t>Modificari programari in trecut</t>
+  </si>
+  <si>
+    <t>Vizualizare calendar</t>
+  </si>
+  <si>
+    <t>Creare programari alti specialisti</t>
+  </si>
+  <si>
+    <t>Modificari programari in viitor alti specialisti</t>
+  </si>
+  <si>
+    <t>Modificari programari in trecut alti specialisti</t>
+  </si>
+  <si>
+    <t>Date de contact clienti</t>
+  </si>
+  <si>
+    <t>Vizualizare baza de date clienti</t>
+  </si>
+  <si>
+    <t>Editare informatii clienti</t>
+  </si>
+  <si>
+    <t>Setari orar</t>
+  </si>
+  <si>
+    <t>Setari exceptii</t>
   </si>
 </sst>
 </file>
@@ -973,7 +985,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
@@ -1172,7 +1184,6 @@
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -1263,10 +1274,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,10 +1475,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.663967611336"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1539,11 +1548,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,9 +1730,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,9 +1830,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
-  </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
@@ -1982,13 +1986,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.24696356275304"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2113,12 +2116,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2602040816326"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2320,9 +2321,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">

</xml_diff>

<commit_message>
new account details for api tests
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cont adminstrator" sheetId="1" state="visible" r:id="rId2"/>
@@ -157,6 +157,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -293,6 +294,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -429,6 +431,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -626,7 +629,7 @@
     <t>Scoala particulara Little piggie</t>
   </si>
   <si>
-    <t>littlepiglet58@automation.33mail.com</t>
+    <t>littlepigletaqs10@automation.33mail.com</t>
   </si>
   <si>
     <t>str Morariei nr 101</t>
@@ -902,7 +905,7 @@
     <t>Scolpol Maria</t>
   </si>
   <si>
-    <t>marilenajooma26@staffcalendis.33mail.com</t>
+    <t>marilenajooama12@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0264555112</t>
@@ -917,7 +920,7 @@
     <t>Mobutu seseku</t>
   </si>
   <si>
-    <t>ideaforkih2@staffcalendis.33mail.com</t>
+    <t>ideaforkih34@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0264111887</t>
@@ -926,7 +929,7 @@
     <t>Moceal Rapil</t>
   </si>
   <si>
-    <t>boomsie4s2@staffcalendis.33mail.com</t>
+    <t>boomsas11@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>0265444112</t>
@@ -935,7 +938,7 @@
     <t>Spiral Agar</t>
   </si>
   <si>
-    <t>ocarinass2@staffcalendis.33mail.com</t>
+    <t>ocarinatrs3@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t>10:00-21:00</t>
@@ -1268,15 +1271,16 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1475,9 +1479,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,10 +1553,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1730,8 +1736,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,6 +1837,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" s="11" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
@@ -1986,12 +1996,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2110,16 +2121,18 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2321,6 +2334,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">

</xml_diff>

<commit_message>
api excel data input
</commit_message>
<xml_diff>
--- a/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
+++ b/src/test/resources/output/Informatii_necesare_setare_cont_demo_api.xlsx
@@ -176,6 +176,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Cont adminstrator'!$A$1:$A$19</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
@@ -331,6 +332,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Domenii!$A$4:$A$7</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
@@ -486,6 +488,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domenii existente'!$A$1:$Q$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -683,7 +686,7 @@
     <t xml:space="preserve">Scoala particulara Little piggie</t>
   </si>
   <si>
-    <t xml:space="preserve">littlepiglesswt81@automation.33mail.com</t>
+    <t xml:space="preserve">littlepiglesswt811@automation.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">str Morariei nr 101</t>
@@ -728,7 +731,7 @@
     <t xml:space="preserve">Rubarba Mihaelaa</t>
   </si>
   <si>
-    <t xml:space="preserve">lilanna33@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">lilanna3311@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555887</t>
@@ -737,7 +740,7 @@
     <t xml:space="preserve">Venula Mihaila</t>
   </si>
   <si>
-    <t xml:space="preserve">moraritza27@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">moraritza2711@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0261111222</t>
@@ -746,7 +749,7 @@
     <t xml:space="preserve">NilaStefania</t>
   </si>
   <si>
-    <t xml:space="preserve">rimmelplus33@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">rimmelplus3311@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0268774112</t>
@@ -959,7 +962,7 @@
     <t xml:space="preserve">Scolpol Maria</t>
   </si>
   <si>
-    <t xml:space="preserve">marilenajohhjss152@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">marilenajohhjss1521@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264555112</t>
@@ -974,7 +977,7 @@
     <t xml:space="preserve">Mobutu seseku</t>
   </si>
   <si>
-    <t xml:space="preserve">ideaforkih397@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">ideaforkih3971@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0264111887</t>
@@ -983,7 +986,7 @@
     <t xml:space="preserve">Moceal Rapil</t>
   </si>
   <si>
-    <t xml:space="preserve">boomsie4s286@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">boomsie4s2861@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">0265444112</t>
@@ -992,7 +995,7 @@
     <t xml:space="preserve">Spiral Agar</t>
   </si>
   <si>
-    <t xml:space="preserve">ocarinass305@staffcalendis.33mail.com</t>
+    <t xml:space="preserve">ocarinass3051@staffcalendis.33mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">10:00-21:00</t>
@@ -1327,7 +1330,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1529,13 +1532,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="72.5182186234818"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.1619433198381"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
@@ -1611,7 +1614,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1792,7 +1795,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2177,14 +2180,14 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.5991902834008"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.2388663967611"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7651821862348"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="10" min="4" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57085020242915"/>

</xml_diff>